<commit_message>
Look and feel improvements.
</commit_message>
<xml_diff>
--- a/spec/data/Simple.xlsx
+++ b/spec/data/Simple.xlsx
@@ -468,7 +468,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -491,6 +491,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
+      <c r="A3">
+        <f>SUM(B1:B10)</f>
+        <v>55</v>
+      </c>
       <c r="B3">
         <v>3</v>
       </c>

</xml_diff>